<commit_message>
output stream was added
</commit_message>
<xml_diff>
--- a/src/main/resources/ІТтаКБ. Сем I. Форма навчання  денна.xlsx
+++ b/src/main/resources/ІТтаКБ. Сем I. Форма навчання  денна.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="139">
   <si>
     <t>Затверджую</t>
   </si>
@@ -458,12 +458,16 @@
   </si>
   <si>
     <t>122(3к.)(43ч.)(4.5кр.)</t>
+  </si>
+  <si>
+    <t>OBAMASSS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1063,42 +1067,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4" style="2" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="5.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="4.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="6.5546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="7.44140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="5.33203125" style="2" customWidth="1"/>
-    <col min="11" max="12" width="6.88671875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.5546875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="5.33203125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="7.33203125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="5.44140625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="7.44140625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="7.33203125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="11.109375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="9.88671875" style="2" customWidth="1"/>
-    <col min="21" max="21" width="9.33203125" style="2" customWidth="1"/>
-    <col min="22" max="23" width="5.5546875" style="2" customWidth="1"/>
-    <col min="24" max="24" width="8.109375" style="2" customWidth="1"/>
-    <col min="25" max="25" width="7" style="2" customWidth="1"/>
-    <col min="26" max="26" width="6.109375" style="2" customWidth="1"/>
-    <col min="27" max="27" width="6.33203125" style="2" customWidth="1"/>
-    <col min="28" max="28" width="10.44140625" style="2" customWidth="1"/>
-    <col min="29" max="30" width="5.88671875" style="2" customWidth="1"/>
-    <col min="31" max="31" width="6.109375" style="2" customWidth="1"/>
-    <col min="32" max="32" width="7.6640625" style="2" customWidth="1"/>
-    <col min="33" max="33" width="5.5546875" style="2" customWidth="1"/>
-    <col min="34" max="34" width="9.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="4.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="28.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="19.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="5.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="9.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="4.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="6.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="2" width="5.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="2" width="7.44140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="2" width="5.33203125" collapsed="true"/>
+    <col min="11" max="12" customWidth="true" style="2" width="6.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="2" width="6.5546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="2" width="5.33203125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="2" width="7.33203125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="2" width="5.44140625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="2" width="7.44140625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="2" width="7.33203125" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="2" width="11.109375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="2" width="9.88671875" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="2" width="9.33203125" collapsed="true"/>
+    <col min="22" max="23" customWidth="true" style="2" width="5.5546875" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="2" width="8.109375" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="2" width="7.0" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="2" width="6.109375" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="2" width="6.33203125" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="2" width="10.44140625" collapsed="true"/>
+    <col min="29" max="30" customWidth="true" style="2" width="5.88671875" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" style="2" width="6.109375" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="2" width="7.6640625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="2" width="5.5546875" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="2" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>

</xml_diff>